<commit_message>
CRM-5138 removing service centre details from downloaded file
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Quote_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Quote_Requested_Parts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Booking Id</t>
   </si>
@@ -44,27 +44,6 @@
     <t>Serial Number</t>
   </si>
   <si>
-    <t>Service Center Name</t>
-  </si>
-  <si>
-    <t>Service Center Mobile No</t>
-  </si>
-  <si>
-    <t>Service Center Address</t>
-  </si>
-  <si>
-    <t>Service Center District</t>
-  </si>
-  <si>
-    <t>Service Center Pincode</t>
-  </si>
-  <si>
-    <t>Service Center State</t>
-  </si>
-  <si>
-    <t>Service Center GST Number</t>
-  </si>
-  <si>
     <t>{spare:booking_id}</t>
   </si>
   <si>
@@ -83,24 +62,6 @@
     <t>{spare:serial_number}</t>
   </si>
   <si>
-    <t>{spare:primary_contact_phone_1}</t>
-  </si>
-  <si>
-    <t>{spare:address}</t>
-  </si>
-  <si>
-    <t>{spare:district}</t>
-  </si>
-  <si>
-    <t>{spare:pincode}</t>
-  </si>
-  <si>
-    <t>{spare:state}</t>
-  </si>
-  <si>
-    <t>{spare:gst_no}</t>
-  </si>
-  <si>
     <t>Product Name</t>
   </si>
   <si>
@@ -114,9 +75,6 @@
   </si>
   <si>
     <t>{spare:amount_due}</t>
-  </si>
-  <si>
-    <t>{spare:company_name}</t>
   </si>
   <si>
     <t>{spare:model_number}</t>
@@ -126,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -141,12 +99,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Cambria"/>
       <charset val="1"/>
@@ -154,11 +106,6 @@
     <font>
       <sz val="10"/>
       <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -187,19 +134,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
@@ -564,22 +509,15 @@
     <col min="6" max="6" width="19.88671875" customWidth="1"/>
     <col min="7" max="8" width="19.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" customWidth="1"/>
-    <col min="12" max="12" width="22.5546875" customWidth="1"/>
-    <col min="13" max="13" width="21.5546875" customWidth="1"/>
-    <col min="14" max="14" width="22.88671875" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="24.6640625" customWidth="1"/>
-    <col min="17" max="24" width="8.6640625" customWidth="1"/>
+    <col min="10" max="17" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -597,97 +535,55 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
CRM-5138 - Removed 'Amount paid' column that was coming in downloaded file, also sequence of columns are same in downloaded file as on view
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Spare_Quote_Requested_Parts.xlsx
+++ b/application/controllers/excel-templates/Spare_Quote_Requested_Parts.xlsx
@@ -24,24 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Booking Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Age of Requested</t>
-  </si>
-  <si>
-    <t>Parts Code</t>
-  </si>
-  <si>
-    <t>Parts Quantity</t>
-  </si>
-  <si>
-    <t>Model Number</t>
-  </si>
-  <si>
-    <t>Serial Number</t>
   </si>
   <si>
     <t>{spare:booking_id}</t>
@@ -62,22 +47,31 @@
     <t>{spare:serial_number}</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
     <t>{spare:services}</t>
   </si>
   <si>
-    <t>Part Requested</t>
+    <t>{spare:model_number}</t>
   </si>
   <si>
-    <t>Amount Due</t>
+    <t>Booking ID</t>
   </si>
   <si>
-    <t>{spare:amount_due}</t>
+    <t>Appliance</t>
   </si>
   <si>
-    <t>{spare:model_number}</t>
+    <t>Spare Part</t>
+  </si>
+  <si>
+    <t>Parts Number</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Model No</t>
+  </si>
+  <si>
+    <t>Serial No</t>
   </si>
 </sst>
 </file>
@@ -106,6 +100,7 @@
     <font>
       <sz val="10"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -493,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2"/>
@@ -507,83 +502,77 @@
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="17" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="16" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1570,6 +1559,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>